<commit_message>
aircrafts database file read correctly
</commit_message>
<xml_diff>
--- a/documents/FAA-Aircraft-Char-DB-AC-150-5300-13B-App-2023-09-07.xlsx
+++ b/documents/FAA-Aircraft-Char-DB-AC-150-5300-13B-App-2023-09-07.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\eclipse-2025-09\eclipse-jee-2025-09-R-win32-x86_64\Data-Challenge-2025\src\main\resources\AircraftsDatabase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\eclipse-2025-09\eclipse-jee-2025-09-R-win32-x86_64\Data-Challenge-2025\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A8654-9241-4B81-B2A7-50D783177344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0837C5BC-BA61-41F9-9F19-3AA51B47AC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="433" xr2:uid="{852B0E64-BCCC-407E-85AF-9EDDBE8136BD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="433" activeTab="1" xr2:uid="{852B0E64-BCCC-407E-85AF-9EDDBE8136BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="ACD_Data" sheetId="4" r:id="rId1"/>
-    <sheet name="ACD_Data_old" sheetId="1" r:id="rId2"/>
+    <sheet name="ACD_Data_bob" sheetId="4" r:id="rId1"/>
+    <sheet name="ACD_Data" sheetId="1" r:id="rId2"/>
     <sheet name="Data_Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -6820,7 +6820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EBF2BF-B620-4F36-AAA0-2F706F1E4A91}">
   <dimension ref="A1:L390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -21595,7 +21595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2C235D-FDEC-42F2-8FD4-154978FFF057}">
   <dimension ref="A1:BD390"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -64801,7 +64801,7 @@
       </c>
       <c r="F19" s="34"/>
     </row>
-    <row r="20" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="30" t="s">
         <v>18</v>
       </c>
@@ -65500,15 +65500,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7734E9F98CDED40B2A2459939C03A36" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="714d4ddb00860fb80f0b4a54262f2f80">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2624f4f0-6830-48b6-9c21-80b2613400ca" xmlns:ns3="d337210d-25f7-4ced-91e1-19a0946fcb25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ce1e1c79ebbab3f68054ecb3b8d007b" ns2:_="" ns3:_="">
     <xsd:import namespace="2624f4f0-6830-48b6-9c21-80b2613400ca"/>
@@ -65739,6 +65730,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -65751,14 +65751,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E9CFC5-E3D9-4ED1-BD0E-6DB50CB80DD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BB49D39-0E65-411C-B5F6-D9EAEB639B61}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -65777,6 +65769,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E9CFC5-E3D9-4ED1-BD0E-6DB50CB80DD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15821E26-0416-43DF-8894-FB2498CD7580}">
   <ds:schemaRefs>

</xml_diff>